<commit_message>
1/8 finals with date edit
</commit_message>
<xml_diff>
--- a/fantasyAnalyticsodds_teams.xlsx
+++ b/fantasyAnalyticsodds_teams.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,33 +481,33 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2021-06-26</t>
+          <t>2021-07-06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Wales</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.1807647740440324</v>
+        <v>0.3961661341853035</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5272305909617613</v>
+        <v>0.3067092651757188</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2920046349942063</v>
+        <v>0.2971246006389776</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2530706836616454</v>
+        <v>0.3521476748313809</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4745075318655851</v>
+        <v>0.3169329073482428</v>
       </c>
     </row>
     <row r="3">
@@ -516,243 +516,33 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2021-06-26</t>
+          <t>2021-07-07</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>England</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.6550984597387405</v>
+        <v>0.5524619634322795</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1187365958276467</v>
+        <v>0.1820493708072083</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2261649444336128</v>
+        <v>0.2654886657605121</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5277182036784298</v>
+        <v>0.4778795983689218</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1899785533242347</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2021-06-27</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Czech Republic</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0.5736872443797865</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.1741923087480443</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.2521204468721693</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.4258034213841081</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.1916115396228487</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2021-06-27</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Belgium</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Portugal</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0.3788187372708758</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.3156822810590632</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.3054989816700611</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.3156822810590632</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.2525458248472505</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2021-06-28</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Croatia</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.1586538461538461</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.5769230769230769</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.2644230769230769</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.2115384615384615</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.4532967032967032</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2021-06-28</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>France</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Switzerland</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0.623532726077566</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.1480890224434219</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.2283782514790121</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.5179069637365575</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.1895539487275801</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2021-06-29</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>England</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0.3655957706384709</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.3277755185034567</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.3066287108580724</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.3168496678866748</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.2924766165107768</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2021-06-29</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Sweden</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Ukraine</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>0.3999920597109735</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.2929172621883436</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.3070906781006829</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.3619700008030863</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.2929172621883436</v>
+        <v>0.2207296066369154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>